<commit_message>
updated the SearchAsync Business Licenses
</commit_message>
<xml_diff>
--- a/AutomationPermitPros/TestData/TestData.xlsx
+++ b/AutomationPermitPros/TestData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JaganPambala\source\repos\Demo-PermitPros\AutomationPermitPros\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandeepThalari\PermitProsProject\Demo-PermitPros\AutomationPermitPros\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AF9983-47A9-48B7-BEBA-F9FE94756287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B514AB-0C6A-4450-A581-15FF27E8A7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-405" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestNames" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="255">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -245,9 +245,6 @@
     <t>Elevator</t>
   </si>
   <si>
-    <t>LIC2026006</t>
-  </si>
-  <si>
     <t>Certificate of Occupancy</t>
   </si>
   <si>
@@ -786,13 +783,19 @@
   </si>
   <si>
     <t>Locations_TestData</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>Lic2007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -951,6 +954,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6E6E6E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1049,7 +1059,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1156,6 +1166,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1471,70 +1482,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F34324-9F29-4487-9FEB-A93C89E2F14E}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>251</v>
-      </c>
       <c r="C1" s="26" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1553,17 +1564,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="AP9" sqref="AP9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="22" customWidth="1"/>
     <col min="2" max="3" width="18" style="22" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="21" customWidth="1"/>
     <col min="6" max="8" width="8" style="21" customWidth="1"/>
     <col min="9" max="10" width="15" style="22" customWidth="1"/>
     <col min="11" max="11" width="20" style="22" customWidth="1"/>
@@ -1578,27 +1589,27 @@
     <col min="23" max="23" width="20" style="22" customWidth="1"/>
     <col min="24" max="24" width="14" style="22" customWidth="1"/>
     <col min="25" max="26" width="25" style="22" customWidth="1"/>
-    <col min="27" max="27" width="16.81640625" style="22" customWidth="1"/>
+    <col min="27" max="27" width="16.85546875" style="22" customWidth="1"/>
     <col min="28" max="28" width="16" style="22" customWidth="1"/>
-    <col min="29" max="29" width="18.54296875" style="22" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.453125" style="22" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.81640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.453125" style="22" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.85546875" style="22" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="9" style="22" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7265625" style="22" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20" style="36" customWidth="1"/>
-    <col min="38" max="38" width="21.453125" style="22" customWidth="1"/>
-    <col min="39" max="42" width="24.26953125" style="22" customWidth="1"/>
-    <col min="43" max="43" width="18.1796875" style="22" customWidth="1"/>
-    <col min="44" max="44" width="16.26953125" style="22" customWidth="1"/>
+    <col min="38" max="38" width="21.42578125" style="22" customWidth="1"/>
+    <col min="39" max="42" width="24.28515625" style="22" customWidth="1"/>
+    <col min="43" max="43" width="18.140625" style="22" customWidth="1"/>
+    <col min="44" max="44" width="16.28515625" style="22" customWidth="1"/>
     <col min="45" max="47" width="30" style="22" customWidth="1"/>
-    <col min="48" max="48" width="15.1796875" style="22" customWidth="1"/>
-    <col min="49" max="16384" width="9.1796875" style="22"/>
+    <col min="48" max="48" width="15.140625" style="22" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1606,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>2</v>
@@ -1618,7 +1629,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>5</v>
@@ -1678,34 +1689,34 @@
         <v>23</v>
       </c>
       <c r="AA1" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC1" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="AB1" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AD1" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="AD1" s="23" t="s">
+      <c r="AE1" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="AE1" s="23" t="s">
+      <c r="AF1" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="23" t="s">
+      <c r="AG1" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="AG1" s="23" t="s">
+      <c r="AH1" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="AH1" s="23" t="s">
+      <c r="AI1" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="AI1" s="23" t="s">
+      <c r="AJ1" s="23" t="s">
         <v>194</v>
-      </c>
-      <c r="AJ1" s="23" t="s">
-        <v>195</v>
       </c>
       <c r="AK1" s="10" t="s">
         <v>26</v>
@@ -1717,22 +1728,22 @@
         <v>28</v>
       </c>
       <c r="AN1" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO1" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="AO1" s="24" t="s">
+      <c r="AP1" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="AP1" s="24" t="s">
-        <v>206</v>
-      </c>
       <c r="AQ1" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AR1" s="23" t="s">
         <v>30</v>
       </c>
       <c r="AS1" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AT1" s="23" t="s">
         <v>31</v>
@@ -1744,7 +1755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:48" ht="24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:48" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1833,7 +1844,7 @@
         <v>47</v>
       </c>
       <c r="AQ2" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AR2" s="22" t="s">
         <v>48</v>
@@ -1851,7 +1862,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -1861,8 +1872,8 @@
       <c r="C3" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>50</v>
+      <c r="D3" s="21" t="b">
+        <v>0</v>
       </c>
       <c r="E3" s="16" t="b">
         <v>0</v>
@@ -1871,7 +1882,7 @@
         <v>51</v>
       </c>
       <c r="G3" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>51</v>
@@ -1916,22 +1927,31 @@
         <v>62</v>
       </c>
       <c r="AK3" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="AL3" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="AM3" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN3" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO3" s="40">
+        <v>12345</v>
+      </c>
+      <c r="AP3" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ3" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="AL3" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM3" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ3" s="22" t="s">
+      <c r="AS3" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="AS3" s="22" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
@@ -1939,7 +1959,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>50</v>
@@ -1993,14 +2013,17 @@
       </c>
       <c r="Z4" s="4"/>
       <c r="AK4" s="11"/>
+      <c r="AO4" s="22">
+        <v>12</v>
+      </c>
       <c r="AQ4" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS4" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="AS4" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>71</v>
       </c>
@@ -2051,10 +2074,10 @@
         <v>53</v>
       </c>
       <c r="AQ5" s="22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="E6" s="17"/>
@@ -2081,7 +2104,7 @@
       <c r="Z6" s="4"/>
       <c r="AK6" s="11"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="D7" s="25"/>
@@ -2109,7 +2132,7 @@
       <c r="Z7" s="4"/>
       <c r="AK7" s="11"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="E8" s="17"/>
@@ -2136,7 +2159,7 @@
       <c r="Z8" s="4"/>
       <c r="AK8" s="11"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="E9" s="17"/>
@@ -2163,7 +2186,7 @@
       <c r="Z9" s="4"/>
       <c r="AK9" s="11"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
     </row>
   </sheetData>
@@ -2229,15 +2252,15 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="22" customWidth="1"/>
     <col min="2" max="3" width="18" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" style="21" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="21" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="21" customWidth="1"/>
     <col min="9" max="10" width="15" style="22" customWidth="1"/>
     <col min="11" max="11" width="12" style="22" customWidth="1"/>
     <col min="12" max="12" width="26" style="22" customWidth="1"/>
@@ -2247,28 +2270,28 @@
     <col min="17" max="17" width="20" style="22" customWidth="1"/>
     <col min="18" max="18" width="14" style="22" customWidth="1"/>
     <col min="19" max="24" width="25" style="22" customWidth="1"/>
-    <col min="25" max="25" width="16.81640625" style="22" customWidth="1"/>
-    <col min="26" max="26" width="20.81640625" style="22" customWidth="1"/>
-    <col min="27" max="27" width="22.26953125" style="22" customWidth="1"/>
-    <col min="28" max="28" width="20.7265625" style="22" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" style="22" customWidth="1"/>
+    <col min="26" max="26" width="20.85546875" style="22" customWidth="1"/>
+    <col min="27" max="27" width="22.28515625" style="22" customWidth="1"/>
+    <col min="28" max="28" width="20.7109375" style="22" customWidth="1"/>
     <col min="29" max="29" width="20" style="22" customWidth="1"/>
-    <col min="30" max="30" width="20.26953125" style="22" customWidth="1"/>
-    <col min="31" max="31" width="10.54296875" style="22" customWidth="1"/>
-    <col min="32" max="39" width="27.453125" style="22" customWidth="1"/>
-    <col min="40" max="40" width="25.81640625" style="22" customWidth="1"/>
+    <col min="30" max="30" width="20.28515625" style="22" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" style="22" customWidth="1"/>
+    <col min="32" max="39" width="27.42578125" style="22" customWidth="1"/>
+    <col min="40" max="40" width="25.85546875" style="22" customWidth="1"/>
     <col min="41" max="41" width="20" style="36" customWidth="1"/>
-    <col min="42" max="42" width="21.453125" style="22" customWidth="1"/>
-    <col min="43" max="44" width="24.26953125" style="22" customWidth="1"/>
-    <col min="45" max="45" width="18.1796875" style="22" customWidth="1"/>
-    <col min="46" max="46" width="16.26953125" style="22" customWidth="1"/>
+    <col min="42" max="42" width="21.42578125" style="22" customWidth="1"/>
+    <col min="43" max="44" width="24.28515625" style="22" customWidth="1"/>
+    <col min="45" max="45" width="18.140625" style="22" customWidth="1"/>
+    <col min="46" max="46" width="16.28515625" style="22" customWidth="1"/>
     <col min="47" max="49" width="30" style="22" customWidth="1"/>
-    <col min="50" max="50" width="15.1796875" style="22" customWidth="1"/>
-    <col min="51" max="16384" width="9.1796875" style="22"/>
+    <col min="50" max="50" width="15.140625" style="22" customWidth="1"/>
+    <col min="51" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:50" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D1" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
@@ -2314,12 +2337,12 @@
         <v>5</v>
       </c>
       <c r="AP1" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AQ1" s="33"/>
       <c r="AR1" s="33"/>
     </row>
-    <row r="2" spans="1:50" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:50" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2327,7 +2350,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>2</v>
@@ -2339,106 +2362,106 @@
         <v>4</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>216</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>217</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="P2" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="U2" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="V2" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="T2" s="27" t="s">
-        <v>225</v>
-      </c>
-      <c r="U2" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="V2" s="27" t="s">
+      <c r="W2" s="27" t="s">
         <v>223</v>
-      </c>
-      <c r="W2" s="27" t="s">
-        <v>224</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>23</v>
       </c>
       <c r="Y2" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="Z2" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="AA2" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AB2" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="AB2" s="23" t="s">
+      <c r="AC2" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="AF2" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="AC2" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="AD2" s="23" t="s">
+      <c r="AG2" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="AE2" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="AG2" s="23" t="s">
+      <c r="AH2" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="AH2" s="23" t="s">
+      <c r="AI2" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="AI2" s="23" t="s">
+      <c r="AJ2" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AK2" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="AJ2" s="23" t="s">
+      <c r="AL2" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="AK2" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="AL2" s="23" t="s">
+      <c r="AM2" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="AM2" s="23" t="s">
+      <c r="AN2" s="23" t="s">
         <v>248</v>
-      </c>
-      <c r="AN2" s="23" t="s">
-        <v>249</v>
       </c>
       <c r="AO2" s="10" t="s">
         <v>26</v>
@@ -2447,19 +2470,19 @@
         <v>27</v>
       </c>
       <c r="AQ2" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="AR2" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="AR2" s="24" t="s">
-        <v>206</v>
-      </c>
       <c r="AS2" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AT2" s="23" t="s">
         <v>30</v>
       </c>
       <c r="AU2" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AV2" s="23" t="s">
         <v>31</v>
@@ -2471,7 +2494,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:50" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -2503,7 +2526,7 @@
         <v>38</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
@@ -2514,22 +2537,22 @@
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="R3" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="Q3" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="R3" s="28" t="s">
+      <c r="S3" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="S3" s="28" t="s">
-        <v>234</v>
-      </c>
       <c r="T3" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U3" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2" t="s">
@@ -2545,7 +2568,7 @@
         <v>47</v>
       </c>
       <c r="AS3" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AT3" s="22" t="s">
         <v>48</v>
@@ -2563,9 +2586,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -2613,21 +2636,21 @@
         <v>62</v>
       </c>
       <c r="AO4" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AP4" s="22" t="s">
         <v>52</v>
       </c>
       <c r="AS4" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU4" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="AU4" s="22" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -2682,15 +2705,15 @@
       <c r="X5" s="4"/>
       <c r="AO5" s="11"/>
       <c r="AS5" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU5" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="AU5" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -2734,12 +2757,12 @@
         <v>52</v>
       </c>
       <c r="AS6" s="22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>6</v>
@@ -2783,10 +2806,10 @@
         <v>52</v>
       </c>
       <c r="AS7" s="22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" s="4"/>
       <c r="D8" s="25"/>
@@ -2812,7 +2835,7 @@
       <c r="X8" s="4"/>
       <c r="AO8" s="11"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9" s="4"/>
       <c r="E9" s="17"/>
@@ -2837,7 +2860,7 @@
       <c r="X9" s="4"/>
       <c r="AO9" s="11"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10" s="4"/>
       <c r="E10" s="17"/>
@@ -2862,7 +2885,7 @@
       <c r="X10" s="4"/>
       <c r="AO10" s="11"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
     </row>
   </sheetData>
@@ -2920,7 +2943,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
@@ -2929,24 +2952,24 @@
     <col min="9" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2963,15 +2986,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
         <v>51</v>
@@ -2980,70 +3003,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
         <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
         <v>85</v>
-      </c>
-      <c r="E6" t="s">
-        <v>86</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
         <v>23</v>
       </c>
@@ -3061,561 +3084,561 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="42"/>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="41"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="8" t="s">
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="8" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
+    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="8" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B59" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
+    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="8" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B65" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B66" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B67" t="s">
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="8" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="8" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B74" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B75" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B76" t="s">
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="8" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B79" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B80" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B81" t="s">
+    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A83" s="8" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="6" t="s">
+      <c r="B84" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B84" s="7" t="s">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="6" t="s">
+      <c r="B85" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B85" s="7" t="s">
+    </row>
+    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="6" t="s">
+      <c r="B86" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B86" s="7" t="s">
+    </row>
+    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87" s="6" t="s">
+      <c r="B87" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B87" s="7" t="s">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="6" t="s">
+      <c r="B88" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B88" s="7" t="s">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="6" t="s">
+      <c r="B89" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B89" s="7" t="s">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="6" t="s">
+      <c r="B90" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B90" s="7" t="s">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="6" t="s">
+      <c r="B91" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B91" s="7" t="s">
+    </row>
+    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="8" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="6" t="s">
+      <c r="B94" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B94" s="7" t="s">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="6" t="s">
+      <c r="B95" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B95" s="7" t="s">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="6" t="s">
+      <c r="B96" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B96" s="7" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="6" t="s">
+      <c r="B97" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B97" s="7" t="s">
+    </row>
+    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A99" s="8" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="6" t="s">
+      <c r="B100" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B100" s="7" t="s">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="6" t="s">
+      <c r="B101" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="B101" s="7" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added location module related code
</commit_message>
<xml_diff>
--- a/AutomationPermitPros/TestData/TestData.xlsx
+++ b/AutomationPermitPros/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JaganPambala\source\repos\Demo-PermitPros\AutomationPermitPros\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AF9983-47A9-48B7-BEBA-F9FE94756287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6538E-25CD-4B41-9024-0051FE902200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestNames" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="253">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -650,9 +650,6 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Operations</t>
-  </si>
-  <si>
     <t>Run</t>
   </si>
   <si>
@@ -668,15 +665,6 @@
     <t>LOC_004</t>
   </si>
   <si>
-    <t>Location Number*</t>
-  </si>
-  <si>
-    <t>Legal Name*</t>
-  </si>
-  <si>
-    <t>Date Opened*</t>
-  </si>
-  <si>
     <t>Date Closed</t>
   </si>
   <si>
@@ -701,9 +689,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>Parent Entity*</t>
-  </si>
-  <si>
     <t>select parent Corporation</t>
   </si>
   <si>
@@ -786,13 +771,25 @@
   </si>
   <si>
     <t>Locations_TestData</t>
+  </si>
+  <si>
+    <t>Legal Name</t>
+  </si>
+  <si>
+    <t>Location Number</t>
+  </si>
+  <si>
+    <t>Date Opened</t>
+  </si>
+  <si>
+    <t>Parent Entity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,34 +875,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -952,7 +921,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -999,12 +968,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
       </patternFill>
     </fill>
@@ -1039,17 +1002,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1099,7 +1061,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
@@ -1127,45 +1089,29 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
-    <cellStyle name="Accent5" xfId="7" builtinId="45"/>
+    <cellStyle name="Accent5" xfId="6" builtinId="45"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -1472,7 +1418,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1482,14 +1428,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>251</v>
+      <c r="A1" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>246</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1497,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1508,7 +1454,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1553,9 +1499,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,7 +1534,7 @@
     <col min="34" max="34" width="9" style="22" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.7265625" style="22" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.7265625" style="22" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20" style="36" customWidth="1"/>
+    <col min="37" max="37" width="20" style="31" customWidth="1"/>
     <col min="38" max="38" width="21.453125" style="22" customWidth="1"/>
     <col min="39" max="42" width="24.26953125" style="22" customWidth="1"/>
     <col min="43" max="43" width="18.1796875" style="22" customWidth="1"/>
@@ -1605,8 +1551,8 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>209</v>
+      <c r="C1" s="29" t="s">
+        <v>208</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>2</v>
@@ -1751,10 +1697,10 @@
       <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="32" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -1851,7 +1797,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:48" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -1865,7 +1811,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>51</v>
@@ -2223,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C07928-5F18-48B9-8606-35B4F75E2114}">
-  <dimension ref="A1:AX11"/>
+  <dimension ref="A1:AX10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2256,7 +2202,7 @@
     <col min="31" max="31" width="10.54296875" style="22" customWidth="1"/>
     <col min="32" max="39" width="27.453125" style="22" customWidth="1"/>
     <col min="40" max="40" width="25.81640625" style="22" customWidth="1"/>
-    <col min="41" max="41" width="20" style="36" customWidth="1"/>
+    <col min="41" max="41" width="20" style="31" customWidth="1"/>
     <col min="42" max="42" width="21.453125" style="22" customWidth="1"/>
     <col min="43" max="44" width="24.26953125" style="22" customWidth="1"/>
     <col min="45" max="45" width="18.1796875" style="22" customWidth="1"/>
@@ -2266,363 +2212,373 @@
     <col min="51" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="D1" s="29" t="s">
+    <row r="1" spans="1:50" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30" t="s">
+      <c r="D1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="31" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="32" t="s">
+      <c r="F1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AP1" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
-    </row>
-    <row r="2" spans="1:50" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="I1" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="T1" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="W1" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD1" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="AE1" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG1" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="AK1" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL1" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="AO1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="AQ1" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="AR1" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="AS1" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AU1" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW1" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" ht="24" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS2" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="AT2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX2" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="T2" s="27" t="s">
-        <v>225</v>
-      </c>
-      <c r="U2" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="V2" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="W2" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z2" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="AA2" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB2" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="AC2" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="AD2" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="AE2" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="AG2" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="AH2" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="AI2" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="AJ2" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="AK2" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="AL2" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="AM2" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="AN2" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="AO2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AP2" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ2" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="AR2" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="AS2" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="AT2" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="AU2" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="AV2" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="AW2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX2" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50" ht="24" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q3" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="R3" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="S3" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="T3" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="U3" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AO3" s="10" t="s">
-        <v>46</v>
+      <c r="F3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO3" s="11" t="s">
+        <v>199</v>
       </c>
       <c r="AP3" s="22" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="AS3" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="AT3" s="22" t="s">
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="AU3" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="AV3" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="AW3" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX3" s="22" t="s">
-        <v>48</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="16" t="b">
+      <c r="E4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="H4" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="R4" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="S4" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="X4" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO4" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AP4" s="22" t="s">
-        <v>52</v>
-      </c>
+      <c r="I4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="AO4" s="11"/>
       <c r="AS4" s="22" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AU4" s="22" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.35">
@@ -2633,13 +2589,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>51</v>
@@ -2650,42 +2606,28 @@
       <c r="H5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="AO5" s="11"/>
+      <c r="AP5" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="AS5" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="AU5" s="22" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
@@ -2702,10 +2644,10 @@
         <v>51</v>
       </c>
       <c r="E6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="G6" s="17" t="b">
         <v>0</v>
@@ -2738,30 +2680,13 @@
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>51</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7" s="4"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -2779,17 +2704,10 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="AO7" s="11"/>
-      <c r="AP7" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS7" s="22" t="s">
-        <v>200</v>
-      </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A8"/>
       <c r="B8" s="4"/>
-      <c r="D8" s="25"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -2838,53 +2756,28 @@
       <c r="AO9" s="11"/>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A10"/>
-      <c r="B10" s="4"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="AO10" s="11"/>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="C11" s="4"/>
+      <c r="C10" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" sqref="AS2:AS8" xr:uid="{81F2BDA8-7B0F-4B79-8461-985B8E321FF8}">
+      <formula1>"SUCCESS,ERROR"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS9:AS1048576" xr:uid="{42FEFFBB-6895-4483-8370-F56BA3B695AC}">
+      <formula1>"SUCCESS,ERROR,FOUND,NOTFOUND"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="AC3:AC1000" xr:uid="{7111A8B8-7901-487B-B285-AF1577E0EC61}">
+      <formula1>"Pass,Fail,Skip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorTitle="Invalid Entry" error="Please enter TRUE or FALSE" sqref="D3:H1000" xr:uid="{3A6F7D6E-9ED9-4E7F-8AC6-FD54D1798B27}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid Module" promptTitle="Module Selection" prompt="Select module type" sqref="B3:B1000" xr:uid="{5AC18F19-C020-44C4-9BCC-36B2D836AD7C}">
+      <formula1>"Business License,Location,Staff Licenses,Dashboard"</formula1>
+    </dataValidation>
     <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid Module" promptTitle="Module Selection" prompt="Select module type" sqref="C1:C1048576" xr:uid="{097B3D47-34CB-41A1-A8E3-7A1EE36199CD}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="AS3:AS9" xr:uid="{81F2BDA8-7B0F-4B79-8461-985B8E321FF8}">
-      <formula1>"SUCCESS,ERROR"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS10:AS1048576" xr:uid="{42FEFFBB-6895-4483-8370-F56BA3B695AC}">
-      <formula1>"SUCCESS,ERROR,FOUND,NOTFOUND"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="AC4:AC1001" xr:uid="{7111A8B8-7901-487B-B285-AF1577E0EC61}">
-      <formula1>"Pass,Fail,Skip"</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorTitle="Invalid Entry" error="Please enter TRUE or FALSE" sqref="D4:H1001" xr:uid="{3A6F7D6E-9ED9-4E7F-8AC6-FD54D1798B27}">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid Module" promptTitle="Module Selection" prompt="Select module type" sqref="B4:B1001" xr:uid="{5AC18F19-C020-44C4-9BCC-36B2D836AD7C}">
-      <formula1>"Business License,Location,Staff Licenses,Dashboard"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:W1048576" xr:uid="{F624F6DA-54DB-465B-8F2D-1041BFD16C2E}">
       <formula1>"TRUE,FALSE"</formula1>
@@ -2898,7 +2791,7 @@
           <x14:formula1>
             <xm:f>ValidationLists!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AE1:AE1048576 AR1:AR1048576</xm:sqref>
+          <xm:sqref>AR1:AR1048576 AE1:AE1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" errorTitle="Invalid State" error="Select from the list" xr:uid="{CC1973D3-4281-4998-AAA6-CD938E1492AB}">
           <x14:formula1>
@@ -3068,10 +2961,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="36"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">

</xml_diff>